<commit_message>
checked stock of some parts
</commit_message>
<xml_diff>
--- a/Documents/Electronics_Parts.xlsx
+++ b/Documents/Electronics_Parts.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/dc8eedf6e5c5d253/Documents/GIT/System-Status-Board/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alex\OneDrive\Documents\GIT\System-Status-Board\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1E6B20D5-13BC-4581-A8C3-EC8EA67987FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="183" documentId="8_{1E6B20D5-13BC-4581-A8C3-EC8EA67987FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{9C1740E5-9F02-4897-927E-2A5EF284C828}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="8055" windowWidth="29040" windowHeight="15840" xr2:uid="{000C6428-41C9-4600-840A-D3AF8691688A}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15796" xr2:uid="{000C6428-41C9-4600-840A-D3AF8691688A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="66">
   <si>
     <t xml:space="preserve">DigiKey number </t>
   </si>
@@ -48,14 +48,194 @@
     <t>Number</t>
   </si>
   <si>
-    <t xml:space="preserve">Desinator </t>
+    <t>Number needed</t>
+  </si>
+  <si>
+    <t>TIVA</t>
+  </si>
+  <si>
+    <t>TM4C123GH6PMT7R</t>
+  </si>
+  <si>
+    <t>TM4C123GH6PMT</t>
+  </si>
+  <si>
+    <t>tiva</t>
+  </si>
+  <si>
+    <t>CAP</t>
+  </si>
+  <si>
+    <t>1276-1000-1-ND</t>
+  </si>
+  <si>
+    <t>.1uf cap</t>
+  </si>
+  <si>
+    <t>.1uf</t>
+  </si>
+  <si>
+    <t>2.1 uf cap</t>
+  </si>
+  <si>
+    <t>2.1uf</t>
+  </si>
+  <si>
+    <t>10uf cap</t>
+  </si>
+  <si>
+    <t>1uf cap</t>
+  </si>
+  <si>
+    <t>47pf cap</t>
+  </si>
+  <si>
+    <t>47pf</t>
+  </si>
+  <si>
+    <t>RES</t>
+  </si>
+  <si>
+    <t>RMCF0603JT10K0CT-ND</t>
+  </si>
+  <si>
+    <t>10K Res</t>
+  </si>
+  <si>
+    <t>10K</t>
+  </si>
+  <si>
+    <t>LCD Board</t>
+  </si>
+  <si>
+    <t>LED</t>
+  </si>
+  <si>
+    <t>754-1122-1-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LED </t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Switch</t>
+  </si>
+  <si>
+    <t>CKN9087CT-ND</t>
+  </si>
+  <si>
+    <t>Zigbee</t>
+  </si>
+  <si>
+    <t>-----------------</t>
+  </si>
+  <si>
+    <t>TLV1117LV33DCYR</t>
+  </si>
+  <si>
+    <t>IC</t>
+  </si>
+  <si>
+    <t>296-28778-1-ND</t>
+  </si>
+  <si>
+    <t>IC REG 3.3</t>
+  </si>
+  <si>
+    <t>ADD NEW RES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADD connector </t>
+  </si>
+  <si>
+    <t xml:space="preserve">System statud board </t>
+  </si>
+  <si>
+    <t>296-11654-1-ND</t>
+  </si>
+  <si>
+    <t>CAN IC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAN </t>
+  </si>
+  <si>
+    <t>SN65HVD230DR</t>
+  </si>
+  <si>
+    <t>120 res</t>
+  </si>
+  <si>
+    <t>1M RES</t>
+  </si>
+  <si>
+    <t>1M</t>
+  </si>
+  <si>
+    <t>Size</t>
+  </si>
+  <si>
+    <t>0603</t>
+  </si>
+  <si>
+    <t>P15442CT-ND</t>
+  </si>
+  <si>
+    <t>CAP ALUM POLY HYB 100UF 50V SMD</t>
+  </si>
+  <si>
+    <t>100uf</t>
+  </si>
+  <si>
+    <t>1210</t>
+  </si>
+  <si>
+    <t>100nf cap</t>
+  </si>
+  <si>
+    <t>LMR23610ADDAR</t>
+  </si>
+  <si>
+    <t>IC REG BUCK ADJ 1A SYNC 8SOPWRPD</t>
+  </si>
+  <si>
+    <t>470nf cap</t>
+  </si>
+  <si>
+    <t>Inductor</t>
+  </si>
+  <si>
+    <t>FIXED IND 56UH 1.7A 126 MOHM</t>
+  </si>
+  <si>
+    <t>MSS1048-563MLB</t>
+  </si>
+  <si>
+    <t>56UH</t>
+  </si>
+  <si>
+    <t>75nf cap</t>
+  </si>
+  <si>
+    <t>40.2K Res</t>
+  </si>
+  <si>
+    <t>490-6538-1-ND</t>
+  </si>
+  <si>
+    <t>47uF</t>
+  </si>
+  <si>
+    <t>In stock</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -63,13 +243,43 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -81,13 +291,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -400,41 +620,794 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCB7D79A-6FD4-4016-89D9-FF8E2F5BB8BB}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:H47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H41" sqref="H41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.59765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.53125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.73046875" customWidth="1"/>
+    <col min="6" max="7" width="13.46484375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="G2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4">
+        <v>6</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5">
+        <v>2</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7">
+        <v>3</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9">
+        <v>5</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" t="s">
+        <v>28</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" t="s">
+        <v>28</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" t="s">
+        <v>28</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" t="s">
+        <v>36</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" t="s">
+        <v>42</v>
+      </c>
+      <c r="E14" t="s">
+        <v>28</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" t="s">
+        <v>44</v>
+      </c>
+      <c r="E15">
+        <v>120</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
+        <v>37</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A23" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A24" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C24" t="s">
         <v>0</v>
       </c>
-      <c r="E1" t="s">
+      <c r="D24" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="E24" t="s">
         <v>3</v>
       </c>
+      <c r="F24" t="s">
+        <v>5</v>
+      </c>
+      <c r="G24" t="s">
+        <v>47</v>
+      </c>
+      <c r="H24" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A25" t="s">
+        <v>7</v>
+      </c>
+      <c r="B25" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" t="s">
+        <v>8</v>
+      </c>
+      <c r="D25" t="s">
+        <v>9</v>
+      </c>
+      <c r="F25">
+        <v>1</v>
+      </c>
+      <c r="H25" s="2"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="B26" t="s">
+        <v>10</v>
+      </c>
+      <c r="C26" t="s">
+        <v>11</v>
+      </c>
+      <c r="D26" t="s">
+        <v>12</v>
+      </c>
+      <c r="E26" t="s">
+        <v>13</v>
+      </c>
+      <c r="F26">
+        <v>6</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="H26" s="2"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="B27" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27" t="s">
+        <v>11</v>
+      </c>
+      <c r="D27" t="s">
+        <v>14</v>
+      </c>
+      <c r="E27" t="s">
+        <v>15</v>
+      </c>
+      <c r="F27">
+        <v>2</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="H27" s="2"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="B28" t="s">
+        <v>10</v>
+      </c>
+      <c r="C28" t="s">
+        <v>11</v>
+      </c>
+      <c r="D28" t="s">
+        <v>16</v>
+      </c>
+      <c r="E28" t="s">
+        <v>16</v>
+      </c>
+      <c r="F28">
+        <v>2</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="H28" s="4"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="B29" t="s">
+        <v>10</v>
+      </c>
+      <c r="C29" t="s">
+        <v>11</v>
+      </c>
+      <c r="D29" t="s">
+        <v>17</v>
+      </c>
+      <c r="E29" t="s">
+        <v>17</v>
+      </c>
+      <c r="F29">
+        <v>3</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="H29" s="2"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="B30" t="s">
+        <v>10</v>
+      </c>
+      <c r="C30" t="s">
+        <v>11</v>
+      </c>
+      <c r="D30" t="s">
+        <v>18</v>
+      </c>
+      <c r="E30" t="s">
+        <v>19</v>
+      </c>
+      <c r="F30">
+        <v>1</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="H30" s="2"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="B31" t="s">
+        <v>20</v>
+      </c>
+      <c r="C31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D31" t="s">
+        <v>22</v>
+      </c>
+      <c r="E31" t="s">
+        <v>23</v>
+      </c>
+      <c r="F31">
+        <v>6</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="H31" s="2"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="B32" t="s">
+        <v>25</v>
+      </c>
+      <c r="C32" t="s">
+        <v>26</v>
+      </c>
+      <c r="D32" t="s">
+        <v>27</v>
+      </c>
+      <c r="E32" t="s">
+        <v>28</v>
+      </c>
+      <c r="F32">
+        <v>1</v>
+      </c>
+      <c r="H32" s="2"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="B33" t="s">
+        <v>29</v>
+      </c>
+      <c r="C33" t="s">
+        <v>30</v>
+      </c>
+      <c r="D33" t="s">
+        <v>29</v>
+      </c>
+      <c r="E33" t="s">
+        <v>28</v>
+      </c>
+      <c r="F33">
+        <v>1</v>
+      </c>
+      <c r="H33" s="2"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="B34" t="s">
+        <v>31</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D34" t="s">
+        <v>31</v>
+      </c>
+      <c r="E34" t="s">
+        <v>28</v>
+      </c>
+      <c r="F34">
+        <v>1</v>
+      </c>
+      <c r="H34" s="2"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A35" t="s">
+        <v>33</v>
+      </c>
+      <c r="B35" t="s">
+        <v>34</v>
+      </c>
+      <c r="C35" t="s">
+        <v>35</v>
+      </c>
+      <c r="D35" t="s">
+        <v>36</v>
+      </c>
+      <c r="F35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A36" t="s">
+        <v>43</v>
+      </c>
+      <c r="B36" t="s">
+        <v>41</v>
+      </c>
+      <c r="C36" t="s">
+        <v>40</v>
+      </c>
+      <c r="D36" t="s">
+        <v>42</v>
+      </c>
+      <c r="E36" t="s">
+        <v>28</v>
+      </c>
+      <c r="F36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="B37" t="s">
+        <v>20</v>
+      </c>
+      <c r="C37" t="s">
+        <v>21</v>
+      </c>
+      <c r="D37" t="s">
+        <v>44</v>
+      </c>
+      <c r="E37">
+        <v>120</v>
+      </c>
+      <c r="F37">
+        <v>1</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="H37" s="2"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="B38" t="s">
+        <v>20</v>
+      </c>
+      <c r="C38" t="s">
+        <v>21</v>
+      </c>
+      <c r="D38" t="s">
+        <v>45</v>
+      </c>
+      <c r="E38" t="s">
+        <v>46</v>
+      </c>
+      <c r="F38">
+        <v>4</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="H38" s="2"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="B39" t="s">
+        <v>10</v>
+      </c>
+      <c r="C39" t="s">
+        <v>49</v>
+      </c>
+      <c r="D39" t="s">
+        <v>50</v>
+      </c>
+      <c r="E39" t="s">
+        <v>51</v>
+      </c>
+      <c r="F39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="B40" t="s">
+        <v>10</v>
+      </c>
+      <c r="C40" t="s">
+        <v>11</v>
+      </c>
+      <c r="D40" t="s">
+        <v>16</v>
+      </c>
+      <c r="E40" t="s">
+        <v>16</v>
+      </c>
+      <c r="F40">
+        <v>1</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="H40" s="2"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="B41" t="s">
+        <v>10</v>
+      </c>
+      <c r="C41" t="s">
+        <v>11</v>
+      </c>
+      <c r="D41" t="s">
+        <v>53</v>
+      </c>
+      <c r="E41" t="s">
+        <v>53</v>
+      </c>
+      <c r="F41">
+        <v>1</v>
+      </c>
+      <c r="G41" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="H41" s="2"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A42" t="s">
+        <v>54</v>
+      </c>
+      <c r="B42" t="s">
+        <v>34</v>
+      </c>
+      <c r="C42" t="s">
+        <v>54</v>
+      </c>
+      <c r="D42" t="s">
+        <v>55</v>
+      </c>
+      <c r="E42" t="s">
+        <v>28</v>
+      </c>
+      <c r="F42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="B43" t="s">
+        <v>10</v>
+      </c>
+      <c r="C43" t="s">
+        <v>11</v>
+      </c>
+      <c r="D43" t="s">
+        <v>56</v>
+      </c>
+      <c r="E43" t="s">
+        <v>56</v>
+      </c>
+      <c r="F43">
+        <v>1</v>
+      </c>
+      <c r="G43" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="B44" t="s">
+        <v>57</v>
+      </c>
+      <c r="C44" t="s">
+        <v>59</v>
+      </c>
+      <c r="D44" t="s">
+        <v>58</v>
+      </c>
+      <c r="E44" t="s">
+        <v>60</v>
+      </c>
+      <c r="F44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="B45" t="s">
+        <v>10</v>
+      </c>
+      <c r="C45" t="s">
+        <v>11</v>
+      </c>
+      <c r="D45" t="s">
+        <v>61</v>
+      </c>
+      <c r="E45" t="s">
+        <v>61</v>
+      </c>
+      <c r="F45">
+        <v>1</v>
+      </c>
+      <c r="G45" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="B46" t="s">
+        <v>20</v>
+      </c>
+      <c r="C46" t="s">
+        <v>21</v>
+      </c>
+      <c r="D46" t="s">
+        <v>62</v>
+      </c>
+      <c r="E46" t="s">
+        <v>62</v>
+      </c>
+      <c r="F46">
+        <v>1</v>
+      </c>
+      <c r="G46">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="B47" t="s">
+        <v>10</v>
+      </c>
+      <c r="C47" t="s">
+        <v>63</v>
+      </c>
+      <c r="D47" t="s">
+        <v>64</v>
+      </c>
+      <c r="E47" t="s">
+        <v>64</v>
+      </c>
+      <c r="F47">
+        <v>2</v>
+      </c>
+      <c r="G47">
+        <v>1210</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>